<commit_message>
Thêm chức năng Import Student
</commit_message>
<xml_diff>
--- a/public/templates/excel/template_import_student.xlsx
+++ b/public/templates/excel/template_import_student.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="733">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="642">
   <si>
     <t>MSSV</t>
   </si>
@@ -1949,280 +1949,7 @@
     <t>6N/1, Ngô Tất Tố, 22, Q Bình Thạnh, TP. Hồ Chí Minh</t>
   </si>
   <si>
-    <t>2015 - 2019</t>
-  </si>
-  <si>
-    <t>2016 - 2019</t>
-  </si>
-  <si>
-    <t>2017 - 2019</t>
-  </si>
-  <si>
-    <t>2018 - 2019</t>
-  </si>
-  <si>
-    <t>2019 - 2019</t>
-  </si>
-  <si>
-    <t>2020 - 2019</t>
-  </si>
-  <si>
-    <t>2021 - 2019</t>
-  </si>
-  <si>
-    <t>2022 - 2019</t>
-  </si>
-  <si>
-    <t>2023 - 2019</t>
-  </si>
-  <si>
-    <t>2024 - 2019</t>
-  </si>
-  <si>
-    <t>2025 - 2019</t>
-  </si>
-  <si>
-    <t>2026 - 2019</t>
-  </si>
-  <si>
-    <t>2027 - 2019</t>
-  </si>
-  <si>
-    <t>2028 - 2019</t>
-  </si>
-  <si>
-    <t>2029 - 2019</t>
-  </si>
-  <si>
-    <t>2030 - 2019</t>
-  </si>
-  <si>
-    <t>2031 - 2019</t>
-  </si>
-  <si>
-    <t>2032 - 2019</t>
-  </si>
-  <si>
-    <t>2033 - 2019</t>
-  </si>
-  <si>
-    <t>2034 - 2019</t>
-  </si>
-  <si>
-    <t>2035 - 2019</t>
-  </si>
-  <si>
-    <t>2036 - 2019</t>
-  </si>
-  <si>
-    <t>2037 - 2019</t>
-  </si>
-  <si>
-    <t>2038 - 2019</t>
-  </si>
-  <si>
-    <t>2039 - 2019</t>
-  </si>
-  <si>
-    <t>2040 - 2019</t>
-  </si>
-  <si>
-    <t>2041 - 2019</t>
-  </si>
-  <si>
-    <t>2042 - 2019</t>
-  </si>
-  <si>
-    <t>2043 - 2019</t>
-  </si>
-  <si>
-    <t>2044 - 2019</t>
-  </si>
-  <si>
-    <t>2045 - 2019</t>
-  </si>
-  <si>
-    <t>2046 - 2019</t>
-  </si>
-  <si>
-    <t>2047 - 2019</t>
-  </si>
-  <si>
-    <t>2048 - 2019</t>
-  </si>
-  <si>
-    <t>2049 - 2019</t>
-  </si>
-  <si>
-    <t>2050 - 2019</t>
-  </si>
-  <si>
-    <t>2051 - 2019</t>
-  </si>
-  <si>
-    <t>2052 - 2019</t>
-  </si>
-  <si>
-    <t>2053 - 2019</t>
-  </si>
-  <si>
-    <t>2054 - 2019</t>
-  </si>
-  <si>
-    <t>2055 - 2019</t>
-  </si>
-  <si>
-    <t>2056 - 2019</t>
-  </si>
-  <si>
-    <t>2057 - 2019</t>
-  </si>
-  <si>
-    <t>2058 - 2019</t>
-  </si>
-  <si>
-    <t>2059 - 2019</t>
-  </si>
-  <si>
-    <t>2060 - 2019</t>
-  </si>
-  <si>
-    <t>2061 - 2019</t>
-  </si>
-  <si>
-    <t>2062 - 2019</t>
-  </si>
-  <si>
-    <t>2063 - 2019</t>
-  </si>
-  <si>
-    <t>2064 - 2019</t>
-  </si>
-  <si>
-    <t>2065 - 2019</t>
-  </si>
-  <si>
-    <t>2066 - 2019</t>
-  </si>
-  <si>
-    <t>2067 - 2019</t>
-  </si>
-  <si>
-    <t>2068 - 2019</t>
-  </si>
-  <si>
-    <t>2069 - 2019</t>
-  </si>
-  <si>
-    <t>2070 - 2019</t>
-  </si>
-  <si>
-    <t>2071 - 2019</t>
-  </si>
-  <si>
-    <t>2072 - 2019</t>
-  </si>
-  <si>
-    <t>2073 - 2019</t>
-  </si>
-  <si>
-    <t>2074 - 2019</t>
-  </si>
-  <si>
-    <t>2075 - 2019</t>
-  </si>
-  <si>
-    <t>2076 - 2019</t>
-  </si>
-  <si>
-    <t>2077 - 2019</t>
-  </si>
-  <si>
-    <t>2078 - 2019</t>
-  </si>
-  <si>
-    <t>2079 - 2019</t>
-  </si>
-  <si>
-    <t>2080 - 2019</t>
-  </si>
-  <si>
-    <t>2081 - 2019</t>
-  </si>
-  <si>
-    <t>2082 - 2019</t>
-  </si>
-  <si>
-    <t>2083 - 2019</t>
-  </si>
-  <si>
-    <t>2084 - 2019</t>
-  </si>
-  <si>
-    <t>2085 - 2019</t>
-  </si>
-  <si>
-    <t>2086 - 2019</t>
-  </si>
-  <si>
-    <t>2087 - 2019</t>
-  </si>
-  <si>
-    <t>2088 - 2019</t>
-  </si>
-  <si>
-    <t>2089 - 2019</t>
-  </si>
-  <si>
-    <t>2090 - 2019</t>
-  </si>
-  <si>
-    <t>2091 - 2019</t>
-  </si>
-  <si>
-    <t>2092 - 2019</t>
-  </si>
-  <si>
-    <t>2093 - 2019</t>
-  </si>
-  <si>
-    <t>2094 - 2019</t>
-  </si>
-  <si>
-    <t>2095 - 2019</t>
-  </si>
-  <si>
-    <t>2096 - 2019</t>
-  </si>
-  <si>
-    <t>2097 - 2019</t>
-  </si>
-  <si>
-    <t>2098 - 2019</t>
-  </si>
-  <si>
-    <t>2099 - 2019</t>
-  </si>
-  <si>
-    <t>2100 - 2019</t>
-  </si>
-  <si>
-    <t>2101 - 2019</t>
-  </si>
-  <si>
-    <t>2102 - 2019</t>
-  </si>
-  <si>
-    <t>2103 - 2019</t>
-  </si>
-  <si>
-    <t>2104 - 2019</t>
-  </si>
-  <si>
-    <t>2105 - 2019</t>
-  </si>
-  <si>
-    <t>2106 - 2019</t>
+    <t>K15</t>
   </si>
 </sst>
 </file>
@@ -2588,7 +2315,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2702,7 +2431,7 @@
         <v>26</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="K3" s="4">
         <v>151101</v>
@@ -2737,7 +2466,7 @@
         <v>33</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="K4" s="4">
         <v>151101</v>
@@ -2772,7 +2501,7 @@
         <v>40</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="K5" s="4">
         <v>151101</v>
@@ -2807,7 +2536,7 @@
         <v>47</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="K6" s="4">
         <v>151101</v>
@@ -2842,7 +2571,7 @@
         <v>54</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>646</v>
+        <v>641</v>
       </c>
       <c r="K7" s="4">
         <v>151101</v>
@@ -2877,7 +2606,7 @@
         <v>61</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>647</v>
+        <v>641</v>
       </c>
       <c r="K8" s="4">
         <v>151101</v>
@@ -2912,7 +2641,7 @@
         <v>68</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>648</v>
+        <v>641</v>
       </c>
       <c r="K9" s="4">
         <v>151101</v>
@@ -2947,7 +2676,7 @@
         <v>73</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>649</v>
+        <v>641</v>
       </c>
       <c r="K10" s="4">
         <v>151101</v>
@@ -2982,7 +2711,7 @@
         <v>81</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="K11" s="4">
         <v>151101</v>
@@ -3017,7 +2746,7 @@
         <v>88</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>651</v>
+        <v>641</v>
       </c>
       <c r="K12" s="4">
         <v>151101</v>
@@ -3050,7 +2779,7 @@
         <v>95</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>652</v>
+        <v>641</v>
       </c>
       <c r="K13" s="4">
         <v>151101</v>
@@ -3085,7 +2814,7 @@
         <v>102</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>653</v>
+        <v>641</v>
       </c>
       <c r="K14" s="4">
         <v>151101</v>
@@ -3120,7 +2849,7 @@
         <v>109</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>654</v>
+        <v>641</v>
       </c>
       <c r="K15" s="4">
         <v>151101</v>
@@ -3155,7 +2884,7 @@
         <v>116</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>655</v>
+        <v>641</v>
       </c>
       <c r="K16" s="4">
         <v>151101</v>
@@ -3190,7 +2919,7 @@
         <v>122</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>656</v>
+        <v>641</v>
       </c>
       <c r="K17" s="4">
         <v>151101</v>
@@ -3225,7 +2954,7 @@
         <v>129</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>657</v>
+        <v>641</v>
       </c>
       <c r="K18" s="4">
         <v>151101</v>
@@ -3258,7 +2987,7 @@
         <v>136</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>658</v>
+        <v>641</v>
       </c>
       <c r="K19" s="4">
         <v>151101</v>
@@ -3291,7 +3020,7 @@
         <v>142</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>659</v>
+        <v>641</v>
       </c>
       <c r="K20" s="4">
         <v>151101</v>
@@ -3326,7 +3055,7 @@
         <v>150</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>660</v>
+        <v>641</v>
       </c>
       <c r="K21" s="4">
         <v>151101</v>
@@ -3361,7 +3090,7 @@
         <v>157</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>661</v>
+        <v>641</v>
       </c>
       <c r="K22" s="4">
         <v>151101</v>
@@ -3396,7 +3125,7 @@
         <v>164</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>662</v>
+        <v>641</v>
       </c>
       <c r="K23" s="4">
         <v>151101</v>
@@ -3431,7 +3160,7 @@
         <v>171</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>663</v>
+        <v>641</v>
       </c>
       <c r="K24" s="4">
         <v>151101</v>
@@ -3466,7 +3195,7 @@
         <v>179</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>664</v>
+        <v>641</v>
       </c>
       <c r="K25" s="4">
         <v>151101</v>
@@ -3501,7 +3230,7 @@
         <v>186</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>665</v>
+        <v>641</v>
       </c>
       <c r="K26" s="4">
         <v>151101</v>
@@ -3536,7 +3265,7 @@
         <v>193</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>666</v>
+        <v>641</v>
       </c>
       <c r="K27" s="4">
         <v>151101</v>
@@ -3571,7 +3300,7 @@
         <v>200</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>667</v>
+        <v>641</v>
       </c>
       <c r="K28" s="4">
         <v>151101</v>
@@ -3606,7 +3335,7 @@
         <v>205</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>668</v>
+        <v>641</v>
       </c>
       <c r="K29" s="4">
         <v>151101</v>
@@ -3641,7 +3370,7 @@
         <v>213</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>669</v>
+        <v>641</v>
       </c>
       <c r="K30" s="4">
         <v>151101</v>
@@ -3676,7 +3405,7 @@
         <v>219</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>670</v>
+        <v>641</v>
       </c>
       <c r="K31" s="4">
         <v>151101</v>
@@ -3711,7 +3440,7 @@
         <v>227</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>671</v>
+        <v>641</v>
       </c>
       <c r="K32" s="4">
         <v>151101</v>
@@ -3746,7 +3475,7 @@
         <v>234</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>672</v>
+        <v>641</v>
       </c>
       <c r="K33" s="4">
         <v>151101</v>
@@ -3781,7 +3510,7 @@
         <v>242</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>673</v>
+        <v>641</v>
       </c>
       <c r="K34" s="4">
         <v>151101</v>
@@ -3816,7 +3545,7 @@
         <v>250</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>674</v>
+        <v>641</v>
       </c>
       <c r="K35" s="4">
         <v>151101</v>
@@ -3851,7 +3580,7 @@
         <v>258</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>675</v>
+        <v>641</v>
       </c>
       <c r="K36" s="4">
         <v>151101</v>
@@ -3886,7 +3615,7 @@
         <v>265</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>676</v>
+        <v>641</v>
       </c>
       <c r="K37" s="4">
         <v>151101</v>
@@ -3921,7 +3650,7 @@
         <v>272</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>677</v>
+        <v>641</v>
       </c>
       <c r="K38" s="4">
         <v>151101</v>
@@ -3956,7 +3685,7 @@
         <v>279</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>678</v>
+        <v>641</v>
       </c>
       <c r="K39" s="4">
         <v>151101</v>
@@ -3991,7 +3720,7 @@
         <v>285</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>679</v>
+        <v>641</v>
       </c>
       <c r="K40" s="4">
         <v>151101</v>
@@ -4026,7 +3755,7 @@
         <v>290</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>680</v>
+        <v>641</v>
       </c>
       <c r="K41" s="4">
         <v>151101</v>
@@ -4061,7 +3790,7 @@
         <v>296</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>681</v>
+        <v>641</v>
       </c>
       <c r="K42" s="4">
         <v>151101</v>
@@ -4096,7 +3825,7 @@
         <v>303</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>682</v>
+        <v>641</v>
       </c>
       <c r="K43" s="4">
         <v>151101</v>
@@ -4131,7 +3860,7 @@
         <v>310</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>683</v>
+        <v>641</v>
       </c>
       <c r="K44" s="4">
         <v>151101</v>
@@ -4166,7 +3895,7 @@
         <v>318</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>684</v>
+        <v>641</v>
       </c>
       <c r="K45" s="4">
         <v>151101</v>
@@ -4201,7 +3930,7 @@
         <v>326</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>685</v>
+        <v>641</v>
       </c>
       <c r="K46" s="4">
         <v>151101</v>
@@ -4236,7 +3965,7 @@
         <v>331</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>686</v>
+        <v>641</v>
       </c>
       <c r="K47" s="4">
         <v>151101</v>
@@ -4271,7 +4000,7 @@
         <v>338</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>687</v>
+        <v>641</v>
       </c>
       <c r="K48" s="4">
         <v>151101</v>
@@ -4306,7 +4035,7 @@
         <v>345</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>688</v>
+        <v>641</v>
       </c>
       <c r="K49" s="4">
         <v>151101</v>
@@ -4341,7 +4070,7 @@
         <v>352</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>689</v>
+        <v>641</v>
       </c>
       <c r="K50" s="4">
         <v>151101</v>
@@ -4376,7 +4105,7 @@
         <v>358</v>
       </c>
       <c r="J51" s="3" t="s">
-        <v>690</v>
+        <v>641</v>
       </c>
       <c r="K51" s="4">
         <v>151101</v>
@@ -4411,7 +4140,7 @@
         <v>364</v>
       </c>
       <c r="J52" s="3" t="s">
-        <v>691</v>
+        <v>641</v>
       </c>
       <c r="K52" s="4">
         <v>151101</v>
@@ -4446,7 +4175,7 @@
         <v>370</v>
       </c>
       <c r="J53" s="3" t="s">
-        <v>692</v>
+        <v>641</v>
       </c>
       <c r="K53" s="4">
         <v>151101</v>
@@ -4481,7 +4210,7 @@
         <v>377</v>
       </c>
       <c r="J54" s="3" t="s">
-        <v>693</v>
+        <v>641</v>
       </c>
       <c r="K54" s="4">
         <v>151101</v>
@@ -4516,7 +4245,7 @@
         <v>384</v>
       </c>
       <c r="J55" s="3" t="s">
-        <v>694</v>
+        <v>641</v>
       </c>
       <c r="K55" s="4">
         <v>151101</v>
@@ -4551,7 +4280,7 @@
         <v>391</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>695</v>
+        <v>641</v>
       </c>
       <c r="K56" s="4">
         <v>151101</v>
@@ -4586,7 +4315,7 @@
         <v>399</v>
       </c>
       <c r="J57" s="3" t="s">
-        <v>696</v>
+        <v>641</v>
       </c>
       <c r="K57" s="4">
         <v>151101</v>
@@ -4621,7 +4350,7 @@
         <v>406</v>
       </c>
       <c r="J58" s="3" t="s">
-        <v>697</v>
+        <v>641</v>
       </c>
       <c r="K58" s="4">
         <v>151101</v>
@@ -4656,7 +4385,7 @@
         <v>412</v>
       </c>
       <c r="J59" s="3" t="s">
-        <v>698</v>
+        <v>641</v>
       </c>
       <c r="K59" s="4">
         <v>151101</v>
@@ -4691,7 +4420,7 @@
         <v>420</v>
       </c>
       <c r="J60" s="3" t="s">
-        <v>699</v>
+        <v>641</v>
       </c>
       <c r="K60" s="4">
         <v>151101</v>
@@ -4726,7 +4455,7 @@
         <v>426</v>
       </c>
       <c r="J61" s="3" t="s">
-        <v>700</v>
+        <v>641</v>
       </c>
       <c r="K61" s="4">
         <v>151101</v>
@@ -4761,7 +4490,7 @@
         <v>432</v>
       </c>
       <c r="J62" s="3" t="s">
-        <v>701</v>
+        <v>641</v>
       </c>
       <c r="K62" s="4">
         <v>151101</v>
@@ -4796,7 +4525,7 @@
         <v>439</v>
       </c>
       <c r="J63" s="3" t="s">
-        <v>702</v>
+        <v>641</v>
       </c>
       <c r="K63" s="4">
         <v>151101</v>
@@ -4831,7 +4560,7 @@
         <v>447</v>
       </c>
       <c r="J64" s="3" t="s">
-        <v>703</v>
+        <v>641</v>
       </c>
       <c r="K64" s="4">
         <v>151101</v>
@@ -4866,7 +4595,7 @@
         <v>454</v>
       </c>
       <c r="J65" s="3" t="s">
-        <v>704</v>
+        <v>641</v>
       </c>
       <c r="K65" s="4">
         <v>151101</v>
@@ -4901,7 +4630,7 @@
         <v>462</v>
       </c>
       <c r="J66" s="3" t="s">
-        <v>705</v>
+        <v>641</v>
       </c>
       <c r="K66" s="4">
         <v>151101</v>
@@ -4936,7 +4665,7 @@
         <v>469</v>
       </c>
       <c r="J67" s="3" t="s">
-        <v>706</v>
+        <v>641</v>
       </c>
       <c r="K67" s="4">
         <v>151101</v>
@@ -4971,7 +4700,7 @@
         <v>476</v>
       </c>
       <c r="J68" s="3" t="s">
-        <v>707</v>
+        <v>641</v>
       </c>
       <c r="K68" s="4">
         <v>151101</v>
@@ -5006,7 +4735,7 @@
         <v>482</v>
       </c>
       <c r="J69" s="3" t="s">
-        <v>708</v>
+        <v>641</v>
       </c>
       <c r="K69" s="4">
         <v>151101</v>
@@ -5041,7 +4770,7 @@
         <v>489</v>
       </c>
       <c r="J70" s="3" t="s">
-        <v>709</v>
+        <v>641</v>
       </c>
       <c r="K70" s="4">
         <v>151101</v>
@@ -5076,7 +4805,7 @@
         <v>495</v>
       </c>
       <c r="J71" s="3" t="s">
-        <v>710</v>
+        <v>641</v>
       </c>
       <c r="K71" s="4">
         <v>151101</v>
@@ -5111,7 +4840,7 @@
         <v>502</v>
       </c>
       <c r="J72" s="3" t="s">
-        <v>711</v>
+        <v>641</v>
       </c>
       <c r="K72" s="4">
         <v>151101</v>
@@ -5146,7 +4875,7 @@
         <v>510</v>
       </c>
       <c r="J73" s="3" t="s">
-        <v>712</v>
+        <v>641</v>
       </c>
       <c r="K73" s="4">
         <v>151101</v>
@@ -5181,7 +4910,7 @@
         <v>517</v>
       </c>
       <c r="J74" s="3" t="s">
-        <v>713</v>
+        <v>641</v>
       </c>
       <c r="K74" s="4">
         <v>151101</v>
@@ -5216,7 +4945,7 @@
         <v>523</v>
       </c>
       <c r="J75" s="3" t="s">
-        <v>714</v>
+        <v>641</v>
       </c>
       <c r="K75" s="4">
         <v>151101</v>
@@ -5251,7 +4980,7 @@
         <v>529</v>
       </c>
       <c r="J76" s="3" t="s">
-        <v>715</v>
+        <v>641</v>
       </c>
       <c r="K76" s="4">
         <v>151101</v>
@@ -5286,7 +5015,7 @@
         <v>535</v>
       </c>
       <c r="J77" s="3" t="s">
-        <v>716</v>
+        <v>641</v>
       </c>
       <c r="K77" s="4">
         <v>151101</v>
@@ -5321,7 +5050,7 @@
         <v>542</v>
       </c>
       <c r="J78" s="3" t="s">
-        <v>717</v>
+        <v>641</v>
       </c>
       <c r="K78" s="4">
         <v>151101</v>
@@ -5356,7 +5085,7 @@
         <v>548</v>
       </c>
       <c r="J79" s="3" t="s">
-        <v>718</v>
+        <v>641</v>
       </c>
       <c r="K79" s="4">
         <v>151101</v>
@@ -5391,7 +5120,7 @@
         <v>555</v>
       </c>
       <c r="J80" s="3" t="s">
-        <v>719</v>
+        <v>641</v>
       </c>
       <c r="K80" s="4">
         <v>151101</v>
@@ -5426,7 +5155,7 @@
         <v>562</v>
       </c>
       <c r="J81" s="3" t="s">
-        <v>720</v>
+        <v>641</v>
       </c>
       <c r="K81" s="4">
         <v>151101</v>
@@ -5461,7 +5190,7 @@
         <v>250</v>
       </c>
       <c r="J82" s="3" t="s">
-        <v>721</v>
+        <v>641</v>
       </c>
       <c r="K82" s="4">
         <v>151101</v>
@@ -5496,7 +5225,7 @@
         <v>573</v>
       </c>
       <c r="J83" s="3" t="s">
-        <v>722</v>
+        <v>641</v>
       </c>
       <c r="K83" s="4">
         <v>151101</v>
@@ -5531,7 +5260,7 @@
         <v>579</v>
       </c>
       <c r="J84" s="3" t="s">
-        <v>723</v>
+        <v>641</v>
       </c>
       <c r="K84" s="4">
         <v>151101</v>
@@ -5566,7 +5295,7 @@
         <v>586</v>
       </c>
       <c r="J85" s="3" t="s">
-        <v>724</v>
+        <v>641</v>
       </c>
       <c r="K85" s="4">
         <v>151101</v>
@@ -5601,7 +5330,7 @@
         <v>593</v>
       </c>
       <c r="J86" s="3" t="s">
-        <v>725</v>
+        <v>641</v>
       </c>
       <c r="K86" s="4">
         <v>151101</v>
@@ -5636,7 +5365,7 @@
         <v>598</v>
       </c>
       <c r="J87" s="3" t="s">
-        <v>726</v>
+        <v>641</v>
       </c>
       <c r="K87" s="4">
         <v>151101</v>
@@ -5671,7 +5400,7 @@
         <v>605</v>
       </c>
       <c r="J88" s="3" t="s">
-        <v>727</v>
+        <v>641</v>
       </c>
       <c r="K88" s="4">
         <v>151101</v>
@@ -5706,7 +5435,7 @@
         <v>612</v>
       </c>
       <c r="J89" s="3" t="s">
-        <v>728</v>
+        <v>641</v>
       </c>
       <c r="K89" s="4">
         <v>151101</v>
@@ -5741,7 +5470,7 @@
         <v>619</v>
       </c>
       <c r="J90" s="3" t="s">
-        <v>729</v>
+        <v>641</v>
       </c>
       <c r="K90" s="4">
         <v>151101</v>
@@ -5776,7 +5505,7 @@
         <v>626</v>
       </c>
       <c r="J91" s="3" t="s">
-        <v>730</v>
+        <v>641</v>
       </c>
       <c r="K91" s="4">
         <v>151101</v>
@@ -5811,7 +5540,7 @@
         <v>633</v>
       </c>
       <c r="J92" s="3" t="s">
-        <v>731</v>
+        <v>641</v>
       </c>
       <c r="K92" s="4">
         <v>151101</v>
@@ -5846,7 +5575,7 @@
         <v>640</v>
       </c>
       <c r="J93" s="3" t="s">
-        <v>732</v>
+        <v>641</v>
       </c>
       <c r="K93" s="4">
         <v>151101</v>

</xml_diff>